<commit_message>
Update output observations file
</commit_message>
<xml_diff>
--- a/AquatoxBasedOptimization/OutputObservations.xlsx
+++ b/AquatoxBasedOptimization/OutputObservations.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21705"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_5EECA2CB5D97A97C2340E1EB3106497128E65A43" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanry\Documents\Repositories\AquatoxBasedOptimization\AquatoxBasedOptimization\AquatoxBasedOptimization\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBBBF54-2BA4-4B0B-A266-A07AE69F950F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report results" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -144,7 +148,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
+    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -174,12 +178,16 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -198,7 +206,7 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Site name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Site ID number"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Sampling time"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Sampling time" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sample depth"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Chlorophyll a µg/l"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Dissolved oxygen mg/l"/>
@@ -507,20 +515,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1045"/>
+  <dimension ref="A1:I1044"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="1" max="2" width="15.68359375" customWidth="1"/>
+    <col min="3" max="3" width="15.578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.68359375" customWidth="1"/>
+    <col min="5" max="5" width="18.15625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" customWidth="1"/>
-    <col min="9" max="9" width="32.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.41796875" customWidth="1"/>
+    <col min="8" max="8" width="28.26171875" customWidth="1"/>
+    <col min="9" max="9" width="32.26171875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -530,7 +540,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -25582,13 +25592,11 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="1045" spans="1:7">
-      <c r="C1045" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>